<commit_message>
ll2UTM2MGRS Complete; MGRS2UTM2LL Started
</commit_message>
<xml_diff>
--- a/Artillery/heading ans.xlsx
+++ b/Artillery/heading ans.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RStudio\MyProjects\Artillery\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RStudio\MyProjects\Artillery\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C43134DF-31C5-4BF1-8E1E-F1A58C9F76A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14385"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
   </bookViews>
   <sheets>
-    <sheet name="randompoints" sheetId="1" r:id="rId1"/>
+    <sheet name="samplell" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
-  <si>
-    <t>longv</t>
-  </si>
-  <si>
-    <t>latv</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
   <si>
     <t>UTME</t>
   </si>
@@ -36,71 +31,95 @@
     <t>gz</t>
   </si>
   <si>
+    <t>hem</t>
+  </si>
+  <si>
     <t>mgrs</t>
   </si>
   <si>
-    <t>54XVF4947024137</t>
-  </si>
-  <si>
-    <t>49GEJ8354543153</t>
-  </si>
-  <si>
-    <t>18QVM0333449016</t>
-  </si>
-  <si>
-    <t>12PWB0645540630</t>
-  </si>
-  <si>
-    <t>58TCP6002851131</t>
-  </si>
-  <si>
-    <t>15RXK9154185684</t>
-  </si>
-  <si>
-    <t>57JYK4992406847</t>
-  </si>
-  <si>
-    <t>47QLG4524441772</t>
-  </si>
-  <si>
-    <t>22FED9367987530</t>
-  </si>
-  <si>
-    <t>51GVM6002809124</t>
-  </si>
-  <si>
-    <t>48SUH1039984632</t>
-  </si>
-  <si>
-    <t>49EDL6263348738</t>
-  </si>
-  <si>
-    <t>07CER0522894933</t>
+    <t>N</t>
+  </si>
+  <si>
+    <t>28NCF3974826536</t>
+  </si>
+  <si>
+    <t>28RDS1373934073</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>08VMP3704140222</t>
+  </si>
+  <si>
+    <t>51CVM8657556286</t>
+  </si>
+  <si>
+    <t>04GFR9717518452</t>
+  </si>
+  <si>
+    <t>40GES5953851185</t>
+  </si>
+  <si>
+    <t>46GDM7907394776</t>
+  </si>
+  <si>
+    <t>35PQN5345923599</t>
+  </si>
+  <si>
+    <t>30NYL6520200042</t>
+  </si>
+  <si>
+    <t>18KYF7100502406</t>
+  </si>
+  <si>
+    <t>29CMR8584617884</t>
+  </si>
+  <si>
+    <t>05QPA7825164049</t>
+  </si>
+  <si>
+    <t>18NYG6931622799</t>
+  </si>
+  <si>
+    <t>26QME1840170439</t>
   </si>
   <si>
     <t>Heading</t>
   </si>
   <si>
+    <t>Point</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
     <t>NE</t>
   </si>
   <si>
     <t>SW</t>
   </si>
   <si>
-    <t>SE</t>
-  </si>
-  <si>
     <t>NW</t>
+  </si>
+  <si>
+    <t>XXXX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0000000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,7 +181,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -235,6 +254,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -424,7 +449,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.249977111117893"/>
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -582,39 +607,54 @@
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -690,7 +730,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -702,7 +742,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -719,9 +759,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -749,14 +789,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -784,6 +841,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -936,425 +1010,653 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="5"/>
+    <col min="1" max="1" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
+        <v>-107.03</v>
+      </c>
+      <c r="C2" s="6">
+        <v>61.94</v>
+      </c>
+      <c r="D2" s="7">
+        <v>393477</v>
+      </c>
+      <c r="E2" s="8">
+        <v>6869162</v>
+      </c>
+      <c r="F2" s="7">
+        <v>13</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H2" s="10"/>
+      <c r="I2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="5" t="str">
+        <f>"From Point: "&amp;A2&amp;" to Point: "&amp;A3</f>
+        <v>From Point: 1 to Point: 2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <v>-16.440000000000001</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.239999999999995</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="5" t="str">
+        <f t="shared" ref="J3:J21" si="0">"From Point: "&amp;A3&amp;" to Point: "&amp;A4</f>
+        <v>From Point: 2 to Point: 3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7">
+        <v>413739</v>
+      </c>
+      <c r="E4" s="8">
+        <v>3134073</v>
+      </c>
+      <c r="F4" s="7">
+        <v>28</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>From Point: 3 to Point: 4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>162.19999999999999</v>
+      </c>
+      <c r="C5" s="6">
+        <v>-57.13</v>
+      </c>
+      <c r="D5" s="7">
+        <v>330527</v>
+      </c>
+      <c r="E5" s="8">
+        <v>3664664</v>
+      </c>
+      <c r="F5" s="7">
+        <v>58</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>From Point: 4 to Point: 5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6">
+        <v>-136.19</v>
+      </c>
+      <c r="C6" s="6">
+        <v>61.69</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>From Point: 5 to Point: 6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7">
+        <v>486575</v>
+      </c>
+      <c r="E7" s="8">
+        <v>1156286</v>
+      </c>
+      <c r="F7" s="7">
+        <v>51</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>From Point: 6 to Point: 7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6">
+        <v>-76.91</v>
+      </c>
+      <c r="C8" s="6">
+        <v>77.459999999999994</v>
+      </c>
+      <c r="D8" s="7">
+        <v>453714</v>
+      </c>
+      <c r="E8" s="8">
+        <v>8598860</v>
+      </c>
+      <c r="F8" s="7">
+        <v>18</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>From Point: 7 to Point: 8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6">
+        <v>-156.5</v>
+      </c>
+      <c r="C9" s="6">
+        <v>-44.96</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>From Point: 8 to Point: 9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7">
+        <v>559538</v>
+      </c>
+      <c r="E10" s="8">
+        <v>5151185</v>
+      </c>
+      <c r="F10" s="7">
+        <v>40</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>From Point: 9 to Point: 10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6">
+        <v>142.47999999999999</v>
+      </c>
+      <c r="C11" s="6">
+        <v>9.5699999999999896</v>
+      </c>
+      <c r="D11" s="7">
+        <v>662427</v>
+      </c>
+      <c r="E11" s="8">
+        <v>1058220</v>
+      </c>
+      <c r="F11" s="7">
+        <v>54</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>From Point: 10 to Point: 11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6">
+        <v>92.72</v>
+      </c>
+      <c r="C12" s="6">
+        <v>-47.9</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>From Point: 11 to Point: 12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7">
+        <v>753459</v>
+      </c>
+      <c r="E13" s="8">
+        <v>1223599</v>
+      </c>
+      <c r="F13" s="7">
+        <v>35</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>From Point: 12 to Point: 13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6">
+        <v>-125.96</v>
+      </c>
+      <c r="C14" s="6">
+        <v>64.08</v>
+      </c>
+      <c r="D14" s="7">
+        <v>355674</v>
+      </c>
+      <c r="E14" s="8">
+        <v>7109283</v>
+      </c>
+      <c r="F14" s="7">
+        <v>10</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>From Point: 13 to Point: 14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6">
+        <v>-0.61000000000001398</v>
+      </c>
+      <c r="C15" s="6">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>From Point: 14 to Point: 15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="7">
+        <v>771005</v>
+      </c>
+      <c r="E16" s="8">
+        <v>8002406</v>
+      </c>
+      <c r="F16" s="7">
+        <v>18</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>From Point: 15 to Point: 16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6">
+        <v>62.33</v>
+      </c>
+      <c r="C17" s="6">
+        <v>-34.17</v>
+      </c>
+      <c r="D17" s="7">
+        <v>438250</v>
+      </c>
+      <c r="E17" s="8">
+        <v>6218792</v>
+      </c>
+      <c r="F17" s="7">
+        <v>41</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="10"/>
+      <c r="I17" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>From Point: 16 to Point: 17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6">
+        <v>-9.5399999999999903</v>
+      </c>
+      <c r="C18" s="6">
+        <v>-76.42</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J18" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>From Point: 17 to Point: 18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="7">
+        <v>678251</v>
+      </c>
+      <c r="E19" s="8">
+        <v>2064049</v>
+      </c>
+      <c r="F19" s="7">
+        <v>5</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>From Point: 18 to Point: 19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>152.26</v>
-      </c>
-      <c r="B2" s="2">
-        <v>-49.08</v>
-      </c>
-      <c r="C2" s="3">
-        <v>445961</v>
-      </c>
-      <c r="D2" s="7">
-        <v>4563387</v>
-      </c>
-      <c r="E2" s="3">
-        <v>56</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="5" t="s">
+      <c r="B20" s="6">
+        <v>-111.71</v>
+      </c>
+      <c r="C20" s="6">
+        <v>53.88</v>
+      </c>
+      <c r="D20" s="7">
+        <v>453326</v>
+      </c>
+      <c r="E20" s="8">
+        <v>5970404</v>
+      </c>
+      <c r="F20" s="7">
+        <v>12</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="10"/>
+      <c r="I20" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>From Point: 19 to Point: 20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>139.51</v>
-      </c>
-      <c r="B3" s="2">
-        <v>72.31</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="B21" s="6">
+        <v>-72.58</v>
+      </c>
+      <c r="C21" s="6">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>From Point: 20 to Point: 21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3">
-        <v>583545</v>
-      </c>
-      <c r="D4" s="7">
-        <v>4843153</v>
-      </c>
-      <c r="E4" s="3">
-        <v>49</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="B22" s="6">
+        <v>-27.77</v>
+      </c>
+      <c r="C22" s="6">
+        <v>17.82</v>
+      </c>
+      <c r="D22" s="7">
+        <v>418401</v>
+      </c>
+      <c r="E22" s="8">
+        <v>1970439</v>
+      </c>
+      <c r="F22" s="7">
+        <v>26</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>-109.55</v>
-      </c>
-      <c r="B5" s="2">
-        <v>33.33</v>
-      </c>
-      <c r="C5" s="3">
-        <v>634952</v>
-      </c>
-      <c r="D5" s="7">
-        <v>3688810</v>
-      </c>
-      <c r="E5" s="3">
-        <v>12</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>-75.95</v>
-      </c>
-      <c r="B6" s="2">
-        <v>23.95</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3">
-        <v>506455</v>
-      </c>
-      <c r="D7" s="7">
-        <v>1640630</v>
-      </c>
-      <c r="E7" s="3">
-        <v>12</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>-115.57</v>
-      </c>
-      <c r="B8" s="2">
-        <v>45.73</v>
-      </c>
-      <c r="C8" s="3">
-        <v>611265</v>
-      </c>
-      <c r="D8" s="7">
-        <v>5065044</v>
-      </c>
-      <c r="E8" s="3">
-        <v>11</v>
-      </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>163.26</v>
-      </c>
-      <c r="B9" s="2">
-        <v>43.8</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="3">
-        <v>691541</v>
-      </c>
-      <c r="D10" s="7">
-        <v>2985684</v>
-      </c>
-      <c r="E10" s="3">
-        <v>15</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>132.44</v>
-      </c>
-      <c r="B11" s="2">
-        <v>-49.35</v>
-      </c>
-      <c r="C11" s="3">
-        <v>314080</v>
-      </c>
-      <c r="D11" s="7">
-        <v>4530483</v>
-      </c>
-      <c r="E11" s="3">
-        <v>53</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>161.54</v>
-      </c>
-      <c r="B12" s="2">
-        <v>-27.94</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="3">
-        <v>345244</v>
-      </c>
-      <c r="D13" s="7">
-        <v>2641772</v>
-      </c>
-      <c r="E13" s="3">
-        <v>47</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>-65.84</v>
-      </c>
-      <c r="B14" s="2">
-        <v>17.510000000000002</v>
-      </c>
-      <c r="C14" s="3">
-        <v>198429</v>
-      </c>
-      <c r="D14" s="7">
-        <v>1938225</v>
-      </c>
-      <c r="E14" s="3">
-        <v>20</v>
-      </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>-49.53</v>
-      </c>
-      <c r="B15" s="2">
-        <v>-55.15</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="3">
-        <v>460028</v>
-      </c>
-      <c r="D16" s="7">
-        <v>5109124</v>
-      </c>
-      <c r="E16" s="3">
-        <v>51</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>-85.7</v>
-      </c>
-      <c r="B17" s="2">
-        <v>-21.11</v>
-      </c>
-      <c r="C17" s="3">
-        <v>635017</v>
-      </c>
-      <c r="D17" s="7">
-        <v>7665127</v>
-      </c>
-      <c r="E17" s="3">
-        <v>16</v>
-      </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>102.82</v>
-      </c>
-      <c r="B18" s="2">
-        <v>38.69</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="3">
-        <v>462633</v>
-      </c>
-      <c r="D19" s="7">
-        <v>3048738</v>
-      </c>
-      <c r="E19" s="3">
-        <v>49</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>37.33</v>
-      </c>
-      <c r="B20" s="2">
-        <v>3.88</v>
-      </c>
-      <c r="C20" s="3">
-        <v>314568</v>
-      </c>
-      <c r="D20" s="7">
-        <v>429046</v>
-      </c>
-      <c r="E20" s="3">
-        <v>37</v>
-      </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>-140.81</v>
-      </c>
-      <c r="B21" s="2">
-        <v>-75.73</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="4" t="s">
-        <v>18</v>
+      <c r="I22" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>